<commit_message>
fix big on excelfile
</commit_message>
<xml_diff>
--- a/fruitDataset.xlsx
+++ b/fruitDataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdourahmanendiaye/Downloads/IOExcel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8AF8348-85A5-8043-98F7-C596A392C43D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD3A5F4-0DC5-5643-BB54-10DC729D5F6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="20740" windowHeight="11160" xr2:uid="{5E1F4FD2-DAED-4D2D-A7F5-C7257A1F3140}"/>
   </bookViews>
@@ -409,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{422AB390-8CBD-4221-87F9-56D95B618B42}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -701,18 +701,33 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C16" t="n">
-        <v>2000.0</v>
-      </c>
-      <c r="D16" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="E16" t="n">
-        <v>13.0</v>
+      <c r="C16">
+        <v>2000</v>
+      </c>
+      <c r="D16">
+        <v>10</v>
+      </c>
+      <c r="E16">
+        <v>13</v>
       </c>
       <c r="F16">
         <f>D16+E16+C16</f>
-        <v>300</v>
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="C17" t="n">
+        <v>3000.0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="F17">
+        <f>D17+E17+C17</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>